<commit_message>
Absolutly new look and new conception
</commit_message>
<xml_diff>
--- a/slots.xlsx
+++ b/slots.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>data</t>
   </si>
@@ -22,6 +22,15 @@
   </si>
   <si>
     <t xml:space="preserve">godzina do</t>
+  </si>
+  <si>
+    <t>przewodniczacy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nr sali</t>
+  </si>
+  <si>
+    <t>Bereta</t>
   </si>
 </sst>
 </file>
@@ -65,12 +74,13 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,7 +599,9 @@
   <sheetFormatPr defaultColWidth="12.630000000000001" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="17.129999999999999"/>
-    <col customWidth="1" min="2" max="5" width="12.630000000000001"/>
+    <col customWidth="1" min="2" max="3" width="12.630000000000001"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" width="14.140625"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" width="5.7109375"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -602,6 +614,12 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="2">
@@ -613,6 +631,12 @@
       <c r="C2" s="3">
         <v>0.52083333333333337</v>
       </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="4">
@@ -624,6 +648,12 @@
       <c r="C3" s="3">
         <v>0.52083333333333337</v>
       </c>
+      <c r="D3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="4">
@@ -635,6 +665,12 @@
       <c r="C4" s="3">
         <v>0.58333333333333337</v>
       </c>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="4">
@@ -646,6 +682,12 @@
       <c r="C5" s="3">
         <v>0.71875</v>
       </c>
+      <c r="D5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="4">
@@ -657,6 +699,12 @@
       <c r="C6" s="3">
         <v>0.6875</v>
       </c>
+      <c r="D6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="4">
@@ -668,6 +716,12 @@
       <c r="C7" s="3">
         <v>0.53125</v>
       </c>
+      <c r="D7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="4">
@@ -679,6 +733,12 @@
       <c r="C8" s="3">
         <v>0.75</v>
       </c>
+      <c r="D8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="4">
@@ -690,6 +750,12 @@
       <c r="C9" s="3">
         <v>0.47916666666666669</v>
       </c>
+      <c r="D9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="4">
@@ -700,6 +766,12 @@
       </c>
       <c r="C10" s="3">
         <v>0.625</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1"/>

</xml_diff>